<commit_message>
Updatet Project Planner, Added Rapport-file.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52f7e2e34e014da6/Documents/Automatiseringsteknikk 3/Mekatronikk/Luretriks-Slange/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{082870B2-B946-470B-8312-6D7E26C31AE1}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2DFD461-CAFE-487C-9D11-B8F517F0B56C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -602,6 +602,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -614,9 +644,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -643,42 +679,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1115,13 +1115,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1129,69 +1129,69 @@
         <v>42</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="26"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="38"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="28"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="40"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="31"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="43"/>
       <c r="AH2" s="16"/>
-      <c r="AI2" s="18" t="s">
+      <c r="AI2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="19"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
     </row>
     <row r="3" spans="1:67" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1218,13 +1218,13 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1407,338 +1407,338 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="19">
         <v>40</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="19">
         <v>10</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="19">
         <v>40</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36">
+      <c r="F5" s="19"/>
+      <c r="G5" s="20">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="19">
         <v>40</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="19">
         <v>3</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="19">
         <v>40</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36">
+      <c r="F6" s="19"/>
+      <c r="G6" s="20">
         <v>0.7</v>
       </c>
     </row>
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="19">
         <v>41</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="19">
         <v>2</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="19">
         <v>41</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36">
+      <c r="F7" s="19"/>
+      <c r="G7" s="20">
         <v>0.35</v>
       </c>
     </row>
     <row r="8" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="19">
         <v>42</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="19">
         <v>1</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="19">
         <v>42</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36">
+      <c r="F8" s="19"/>
+      <c r="G8" s="20">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="19">
         <v>42</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="19">
         <v>2</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="19">
         <v>42</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36">
-        <v>0.1</v>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20">
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="19">
         <v>43</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="19">
         <v>4</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="19">
         <v>42</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="19">
         <v>1</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="19">
         <v>45</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="19">
         <v>2</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="19">
         <v>45</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="19">
         <v>2</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="19">
         <v>47</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="19">
         <v>2</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Finished movement-code. Need to test when robot is assembled. Updated projectplanner to reflect this work done.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2DFD461-CAFE-487C-9D11-B8F517F0B56C}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAB8A272-B511-4BFC-AE54-AF84697CF890}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="20">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated documents. Added wifi-module to movement-module and combined for Complete program for arduino. Btw, dont use pin 12-17 for servo, this makes the ESP32 crash when trying to parse incoming packets. I do not know why.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAB8A272-B511-4BFC-AE54-AF84697CF890}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{85B73D10-2A00-429E-BB5C-85D13438469B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>PERIODS</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Integrate ImPro/Movement</t>
   </si>
   <si>
-    <t>Deep Learning</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -211,13 +208,64 @@
   </si>
   <si>
     <t>Snake-like Robot</t>
+  </si>
+  <si>
+    <t>Maze</t>
+  </si>
+  <si>
+    <t>Find snake</t>
+  </si>
+  <si>
+    <t>Find target</t>
+  </si>
+  <si>
+    <t>Send commands</t>
+  </si>
+  <si>
+    <t>Collision detect</t>
+  </si>
+  <si>
+    <t>See the maze</t>
+  </si>
+  <si>
+    <t>Pathfinding</t>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>Integrate maze</t>
+  </si>
+  <si>
+    <t>RUBEN/HÅKON</t>
+  </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Controlling</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Build GUI</t>
+  </si>
+  <si>
+    <t>Håkon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -345,8 +393,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +447,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -490,7 +556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,8 +612,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,9 +678,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -680,14 +744,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Forklarende tekst" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="God" xfId="19" builtinId="26"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Overskrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -1089,10 +1166,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO30"/>
+  <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1104,9 +1181,9 @@
     <col min="8" max="27" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:42" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1114,14 +1191,14 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="1:42" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1129,69 +1206,69 @@
         <v>42</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="40"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="41" t="s">
+      <c r="AA2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="43"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="42"/>
       <c r="AH2" s="16"/>
-      <c r="AI2" s="28" t="s">
+      <c r="AI2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="29"/>
-      <c r="AP2" s="29"/>
-    </row>
-    <row r="3" spans="1:67" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="31" t="s">
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+    </row>
+    <row r="3" spans="1:42" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="34" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1206,7 +1283,7 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
+      <c r="R3" s="46"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
@@ -1217,200 +1294,86 @@
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+    <row r="4" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="3">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="I4" s="3">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="J4" s="3">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="K4" s="3">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="L4" s="3">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="N4" s="3">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="O4" s="3">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="P4" s="3">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="3">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="R4" s="3">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="S4" s="3">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="T4" s="3">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="U4" s="3">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="V4" s="3">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="W4" s="3">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="X4" s="3">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="Y4" s="3">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="Z4" s="3">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="AA4" s="3">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="AB4" s="3">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="AC4" s="3">
-        <v>22</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>23</v>
-      </c>
-      <c r="AE4" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AF4" s="3">
-        <v>25</v>
-      </c>
-      <c r="AG4" s="3">
-        <v>26</v>
-      </c>
-      <c r="AH4" s="3">
-        <v>27</v>
-      </c>
-      <c r="AI4" s="3">
-        <v>28</v>
-      </c>
-      <c r="AJ4" s="3">
-        <v>29</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>30</v>
-      </c>
-      <c r="AL4" s="3">
-        <v>31</v>
-      </c>
-      <c r="AM4" s="3">
-        <v>32</v>
-      </c>
-      <c r="AN4" s="3">
-        <v>33</v>
-      </c>
-      <c r="AO4" s="3">
-        <v>34</v>
-      </c>
-      <c r="AP4" s="3">
-        <v>35</v>
-      </c>
-      <c r="AQ4" s="3">
-        <v>36</v>
-      </c>
-      <c r="AR4" s="3">
-        <v>37</v>
-      </c>
-      <c r="AS4" s="3">
-        <v>38</v>
-      </c>
-      <c r="AT4" s="3">
-        <v>39</v>
-      </c>
-      <c r="AU4" s="3">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="3">
-        <v>41</v>
-      </c>
-      <c r="AW4" s="3">
-        <v>42</v>
-      </c>
-      <c r="AX4" s="3">
-        <v>43</v>
-      </c>
-      <c r="AY4" s="3">
-        <v>44</v>
-      </c>
-      <c r="AZ4" s="3">
-        <v>45</v>
-      </c>
-      <c r="BA4" s="3">
-        <v>46</v>
-      </c>
-      <c r="BB4" s="3">
-        <v>47</v>
-      </c>
-      <c r="BC4" s="3">
-        <v>48</v>
-      </c>
-      <c r="BD4" s="3">
-        <v>49</v>
-      </c>
-      <c r="BE4" s="3">
-        <v>50</v>
-      </c>
-      <c r="BF4" s="3">
-        <v>51</v>
-      </c>
-      <c r="BG4" s="3">
-        <v>52</v>
-      </c>
-      <c r="BH4" s="3">
-        <v>53</v>
-      </c>
-      <c r="BI4" s="3">
-        <v>54</v>
-      </c>
-      <c r="BJ4" s="3">
-        <v>55</v>
-      </c>
-      <c r="BK4" s="3">
-        <v>56</v>
-      </c>
-      <c r="BL4" s="3">
-        <v>57</v>
-      </c>
-      <c r="BM4" s="3">
-        <v>58</v>
-      </c>
-      <c r="BN4" s="3">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="19">
@@ -1426,12 +1389,32 @@
       <c r="G5" s="20">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="22" t="s">
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+    </row>
+    <row r="6" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="19">
@@ -1447,12 +1430,32 @@
       <c r="G6" s="20">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+    </row>
+    <row r="7" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="19">
@@ -1466,14 +1469,34 @@
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="20">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="22" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+    </row>
+    <row r="8" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="19">
@@ -1487,14 +1510,34 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="22" t="s">
+        <v>0.35</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+    </row>
+    <row r="9" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="19">
@@ -1510,12 +1553,32 @@
       <c r="G9" s="20">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="22" t="s">
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+    </row>
+    <row r="10" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="19">
@@ -1524,221 +1587,813 @@
       <c r="D10" s="19">
         <v>4</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>20</v>
+      <c r="E10" s="19">
+        <v>42</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="20">
+        <f>AVERAGE(G11:G13)</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+    </row>
+    <row r="11" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="43" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="19">
+        <v>43</v>
+      </c>
+      <c r="D11" s="19">
+        <v>3</v>
+      </c>
+      <c r="E11" s="19">
         <v>42</v>
       </c>
-      <c r="D11" s="19">
+      <c r="F11" s="19"/>
+      <c r="G11" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+    </row>
+    <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="19">
+        <v>46</v>
+      </c>
+      <c r="D12" s="19">
         <v>1</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="19">
-        <v>45</v>
-      </c>
-      <c r="D12" s="19">
-        <v>2</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>22</v>
+      <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+    </row>
+    <row r="13" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="43" t="s">
+        <v>33</v>
       </c>
       <c r="C13" s="19">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="20">
+        <v>0</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+    </row>
+    <row r="14" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="19">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="E14" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="19">
+        <v>42</v>
+      </c>
       <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
+      <c r="G14" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="19">
+        <v>45</v>
+      </c>
+      <c r="D15" s="19">
+        <v>3</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+      <c r="G15" s="20">
+        <f>AVERAGE(G16:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+    </row>
+    <row r="16" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="19">
+        <v>45</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+    </row>
+    <row r="17" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="B17" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="19">
+        <v>46</v>
+      </c>
+      <c r="D17" s="19">
+        <v>1</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="20">
+        <v>0</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+    </row>
+    <row r="18" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
+      <c r="B18" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="19">
+        <v>47</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
+      <c r="G18" s="20">
+        <v>0</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+    </row>
+    <row r="19" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="19">
+        <v>44</v>
+      </c>
+      <c r="D19" s="19">
+        <v>4</v>
+      </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="G19" s="20">
+        <f>AVERAGE(G20:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+    </row>
+    <row r="20" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="19">
+        <v>44</v>
+      </c>
+      <c r="D20" s="19">
+        <v>2</v>
+      </c>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+    </row>
+    <row r="21" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="19">
+        <v>46</v>
+      </c>
+      <c r="D21" s="19">
+        <v>2</v>
+      </c>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
+      <c r="G21" s="20">
+        <v>0</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+    </row>
+    <row r="22" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="19">
+        <v>43</v>
+      </c>
+      <c r="D22" s="19">
+        <v>2</v>
+      </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="G22" s="20">
+        <f>AVERAGE(G23:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+    </row>
+    <row r="23" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="19">
+        <v>43</v>
+      </c>
+      <c r="D23" s="19">
+        <v>1</v>
+      </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
+      <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+    </row>
+    <row r="24" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="19">
+        <v>43</v>
+      </c>
+      <c r="D24" s="19">
+        <v>1</v>
+      </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="G24" s="20">
+        <v>0</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+    </row>
+    <row r="25" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="19">
+        <v>44</v>
+      </c>
+      <c r="D25" s="19">
+        <v>1</v>
+      </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+      <c r="G25" s="20">
+        <v>0</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+    </row>
+    <row r="26" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="19">
+        <v>45</v>
+      </c>
+      <c r="D26" s="19">
+        <v>1</v>
+      </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="G26" s="20">
+        <v>0</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+    </row>
+    <row r="27" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="19">
+        <v>47</v>
+      </c>
+      <c r="D27" s="19">
+        <v>2</v>
+      </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="20">
+        <v>0</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+    </row>
+    <row r="28" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
-      <c r="B28" s="18"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+    </row>
+    <row r="29" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+    </row>
+    <row r="30" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="20"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+    </row>
+    <row r="31" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+    </row>
+    <row r="32" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1756,7 +2411,7 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO30">
+  <conditionalFormatting sqref="H5:AC30">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1782,12 +2437,12 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BO31">
+  <conditionalFormatting sqref="B31:AC31">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="H4:AC4">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated project planner and wrote some documentation in the report concerning communication between ESP32 and PC, as well as between camera-module and python.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{85B73D10-2A00-429E-BB5C-85D13438469B}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D122B32A-6A1C-4717-9312-157B898AA036}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>PERIODS</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Håkon</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
   </si>
 </sst>
 </file>
@@ -693,6 +696,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,18 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1168,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1192,13 +1195,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:42" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1206,69 +1209,69 @@
         <v>42</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="37"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="37"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="41"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="27" t="s">
+      <c r="V2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="39"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="43"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="40" t="s">
+      <c r="AA2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="42"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="46"/>
       <c r="AH2" s="16"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AI2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
     </row>
     <row r="3" spans="1:42" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="38" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1283,7 +1286,7 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="46"/>
+      <c r="R3" s="29"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
@@ -1295,13 +1298,13 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="3">
         <v>39</v>
       </c>
@@ -1510,7 +1513,7 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -1590,7 +1593,7 @@
       <c r="E10" s="19">
         <v>42</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
         <v>1.6666666666666666E-2</v>
@@ -1618,7 +1621,7 @@
     </row>
     <row r="11" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="19">
@@ -1657,7 +1660,7 @@
     </row>
     <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="19">
@@ -1694,7 +1697,7 @@
     </row>
     <row r="13" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="19">
@@ -1747,7 +1750,7 @@
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="20">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -1812,7 +1815,7 @@
     </row>
     <row r="16" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="19">
@@ -1849,7 +1852,7 @@
     </row>
     <row r="17" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="19">
@@ -1886,7 +1889,7 @@
     </row>
     <row r="18" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="19">
@@ -1923,7 +1926,7 @@
     </row>
     <row r="19" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>37</v>
@@ -1937,8 +1940,8 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="20">
-        <f>AVERAGE(G20:G21)</f>
-        <v>0</v>
+        <f>AVERAGE(G20:G22)</f>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -1963,7 +1966,7 @@
     </row>
     <row r="20" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="19">
@@ -2000,7 +2003,7 @@
     </row>
     <row r="21" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="19">
@@ -2036,23 +2039,22 @@
       <c r="AA21"/>
     </row>
     <row r="22" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>42</v>
+      <c r="A22" s="23"/>
+      <c r="B22" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="19">
         <v>43</v>
       </c>
       <c r="D22" s="19">
-        <v>2</v>
-      </c>
-      <c r="E22" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="19">
+        <v>43</v>
+      </c>
       <c r="F22" s="19"/>
       <c r="G22" s="20">
-        <f>AVERAGE(G23:G25)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
@@ -2076,19 +2078,20 @@
       <c r="AA22"/>
     </row>
     <row r="23" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="43" t="s">
-        <v>46</v>
+      <c r="A23" s="23"/>
+      <c r="B23" s="21" t="s">
+        <v>42</v>
       </c>
       <c r="C23" s="19">
         <v>43</v>
       </c>
       <c r="D23" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="20">
+        <f>AVERAGE(G24:G26)</f>
         <v>0</v>
       </c>
       <c r="H23"/>
@@ -2114,8 +2117,8 @@
     </row>
     <row r="24" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="43" t="s">
-        <v>43</v>
+      <c r="B24" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="C24" s="19">
         <v>43</v>
@@ -2151,11 +2154,11 @@
     </row>
     <row r="25" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="43" t="s">
-        <v>44</v>
+      <c r="B25" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="C25" s="19">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
@@ -2187,14 +2190,12 @@
       <c r="AA25"/>
     </row>
     <row r="26" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>45</v>
+      <c r="A26" s="22"/>
+      <c r="B26" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="C26" s="19">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="19">
         <v>1</v>
@@ -2226,22 +2227,24 @@
       <c r="AA26"/>
     </row>
     <row r="27" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>24</v>
+      <c r="A27" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C27" s="19">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="19">
-        <v>2</v>
-      </c>
-      <c r="E27" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="19">
+        <v>43</v>
+      </c>
       <c r="F27" s="19"/>
       <c r="G27" s="20">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -2265,13 +2268,23 @@
       <c r="AA27"/>
     </row>
     <row r="28" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
+      <c r="A28" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="19">
+        <v>47</v>
+      </c>
+      <c r="D28" s="19">
+        <v>2</v>
+      </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="20"/>
+      <c r="G28" s="20">
+        <v>0</v>
+      </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>

</xml_diff>

<commit_message>
Taken some test pictures to filter the maze. Found edges, made lines with algorithm. Sent those lines to the RRT*-function. Updated projectplanner and report.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D122B32A-6A1C-4717-9312-157B898AA036}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16D1CB5C-6E6C-4BF4-ABC5-12226127A0BC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="39" t="s">
@@ -1429,9 +1429,11 @@
       <c r="E6" s="19">
         <v>40</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="19">
+        <v>2</v>
+      </c>
       <c r="G6" s="20">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -1472,7 +1474,7 @@
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="20">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -1513,7 +1515,7 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -1554,7 +1556,7 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="20">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -1596,7 +1598,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>1.6666666666666666E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1635,7 +1637,7 @@
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="20">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -1941,7 +1943,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="20">
         <f>AVERAGE(G20:G22)</f>
-        <v>9.9999999999999992E-2</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -1978,7 +1980,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -2015,7 +2017,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="20">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -2054,7 +2056,7 @@
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="20">
-        <v>0.3</v>
+        <v>0.75</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>

</xml_diff>

<commit_message>
Adjusted the collision-detection in RRT, it now will keep the lines at a minimum of 20 pixels (adjustable in main) from the walls of the maze. Updated the filter in maze-recognizer.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16D1CB5C-6E6C-4BF4-ABC5-12226127A0BC}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{077FD3F5-E004-4BE0-B5A6-FE9814AC5818}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="20">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="20">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -1598,7 +1598,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.13333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="20">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -1943,7 +1943,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="20">
         <f>AVERAGE(G20:G22)</f>
-        <v>0.48333333333333334</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -1980,7 +1980,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="20">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -2017,7 +2017,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="20">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="20">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>

</xml_diff>

<commit_message>
Added pictures for the report. Started working more on the report.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{BCE32247-F1EF-4B75-A979-B61A048AEDEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{077FD3F5-E004-4BE0-B5A6-FE9814AC5818}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>PERIODS</t>
   </si>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="39" t="s">
@@ -1472,9 +1472,11 @@
       <c r="E7" s="19">
         <v>41</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="19">
+        <v>3</v>
+      </c>
       <c r="G7" s="20">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -1513,9 +1515,11 @@
       <c r="E8" s="19">
         <v>42</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="19">
+        <v>2</v>
+      </c>
       <c r="G8" s="20">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -1556,7 +1560,7 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="20">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -1598,7 +1602,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.16666666666666666</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1637,7 +1641,7 @@
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="20">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -1750,9 +1754,11 @@
       <c r="E14" s="19">
         <v>42</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="19">
+        <v>2</v>
+      </c>
       <c r="G14" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -2080,7 +2086,9 @@
       <c r="AA22"/>
     </row>
     <row r="23" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="B23" s="21" t="s">
         <v>42</v>
       </c>
@@ -2246,7 +2254,7 @@
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="20">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>

</xml_diff>

<commit_message>
General spellchecking. Updated Arduino-program to make use of lateral shifts. Updated project planner. Cleaned up Arduino code to remove redundant lines.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69508908-3E05-4171-9C18-B38999568F4D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
   <dimension ref="A1:AP32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="39" t="s">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="20">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1558,9 +1558,11 @@
       <c r="E9" s="19">
         <v>42</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="19">
+        <v>3</v>
+      </c>
       <c r="G9" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -1602,7 +1604,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.26666666666666666</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1639,9 +1641,11 @@
       <c r="E11" s="19">
         <v>42</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="19">
+        <v>2</v>
+      </c>
       <c r="G11" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -1675,10 +1679,14 @@
       <c r="D12" s="19">
         <v>1</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="E12" s="19">
+        <v>44</v>
+      </c>
+      <c r="F12" s="19">
+        <v>1</v>
+      </c>
       <c r="G12" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -1712,10 +1720,12 @@
       <c r="D13" s="19">
         <v>1</v>
       </c>
-      <c r="E13" s="19"/>
+      <c r="E13" s="19">
+        <v>44</v>
+      </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -1794,11 +1804,13 @@
       <c r="D15" s="19">
         <v>3</v>
       </c>
-      <c r="E15" s="19"/>
+      <c r="E15" s="19">
+        <v>44</v>
+      </c>
       <c r="F15" s="19"/>
       <c r="G15" s="20">
         <f>AVERAGE(G16:G18)</f>
-        <v>0</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -1832,10 +1844,14 @@
       <c r="D16" s="19">
         <v>1</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="19">
+        <v>44</v>
+      </c>
+      <c r="F16" s="19">
+        <v>1</v>
+      </c>
       <c r="G16" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
@@ -1869,10 +1885,12 @@
       <c r="D17" s="19">
         <v>1</v>
       </c>
-      <c r="E17" s="19"/>
+      <c r="E17" s="19">
+        <v>44</v>
+      </c>
       <c r="F17" s="19"/>
       <c r="G17" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
@@ -1906,10 +1924,14 @@
       <c r="D18" s="19">
         <v>1</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="19">
+        <v>44</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
       <c r="G18" s="20">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
@@ -1945,11 +1967,13 @@
       <c r="D19" s="19">
         <v>4</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="19">
+        <v>43</v>
+      </c>
       <c r="F19" s="19"/>
       <c r="G19" s="20">
         <f>AVERAGE(G20:G22)</f>
-        <v>0.6333333333333333</v>
+        <v>0.93333333333333324</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -1983,10 +2007,14 @@
       <c r="D20" s="19">
         <v>2</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="E20" s="19">
+        <v>43</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1</v>
+      </c>
       <c r="G20" s="20">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
@@ -2020,10 +2048,14 @@
       <c r="D21" s="19">
         <v>2</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="E21" s="19">
+        <v>43</v>
+      </c>
+      <c r="F21" s="19">
+        <v>2</v>
+      </c>
       <c r="G21" s="20">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -2060,9 +2092,11 @@
       <c r="E22" s="19">
         <v>43</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="19">
+        <v>2</v>
+      </c>
       <c r="G22" s="20">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
@@ -2098,11 +2132,13 @@
       <c r="D23" s="19">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="19">
+        <v>43</v>
+      </c>
       <c r="F23" s="19"/>
       <c r="G23" s="20">
         <f>AVERAGE(G24:G26)</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -2136,10 +2172,12 @@
       <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="19"/>
+      <c r="E24" s="19">
+        <v>43</v>
+      </c>
       <c r="F24" s="19"/>
       <c r="G24" s="20">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2173,10 +2211,12 @@
       <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="19">
+        <v>43</v>
+      </c>
       <c r="F25" s="19"/>
       <c r="G25" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -2210,10 +2250,12 @@
       <c r="D26" s="19">
         <v>1</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="19">
+        <v>43</v>
+      </c>
       <c r="F26" s="19"/>
       <c r="G26" s="20">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -2254,7 +2296,7 @@
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="20">
-        <v>0.65</v>
+        <v>0.9</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -2293,7 +2335,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="20">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>

</xml_diff>

<commit_message>
Added functionality to prepare maze for Seek and Destroy.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69508908-3E05-4171-9C18-B38999568F4D}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E24398F6-4EE2-4B37-BBA7-4398864A6478}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="39" t="s">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="20">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1604,7 +1604,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.71666666666666667</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -1810,7 +1810,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="20">
         <f>AVERAGE(G16:G18)</f>
-        <v>0.79999999999999993</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="20">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
@@ -1931,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
@@ -1970,10 +1970,12 @@
       <c r="E19" s="19">
         <v>43</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="19">
+        <v>4</v>
+      </c>
       <c r="G19" s="20">
         <f>AVERAGE(G20:G22)</f>
-        <v>0.93333333333333324</v>
+        <v>1</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -2055,7 +2057,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -2332,10 +2334,12 @@
       <c r="D28" s="19">
         <v>2</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="19">
+        <v>44</v>
+      </c>
       <c r="F28" s="19"/>
       <c r="G28" s="20">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>

</xml_diff>

<commit_message>
General typo-fixing. Changed some variable names to make more sense.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E24398F6-4EE2-4B37-BBA7-4398864A6478}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAA82BA3-2D24-4E67-9A14-F91BCD9795EC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="39" t="s">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="20">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1604,7 +1604,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.79999999999999993</v>
+        <v>0.93333333333333324</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="20">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -1810,7 +1810,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="20">
         <f>AVERAGE(G16:G18)</f>
-        <v>0.91666666666666663</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="20">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>

</xml_diff>

<commit_message>
Added documentation to every class. Program is considered done.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAA82BA3-2D24-4E67-9A14-F91BCD9795EC}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20C6A4E9-8285-429A-8BAC-37F8D2DA8CF0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,7 +617,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,9 +701,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1171,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1195,13 +1192,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:42" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1209,69 +1206,69 @@
         <v>48</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="40"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="39" t="s">
+      <c r="Q2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="40"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="31" t="s">
+      <c r="V2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="43"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="42"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="44" t="s">
+      <c r="AA2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="46"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="45"/>
       <c r="AH2" s="16"/>
-      <c r="AI2" s="31" t="s">
+      <c r="AI2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
     </row>
     <row r="3" spans="1:42" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1286,7 +1283,7 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="29"/>
+      <c r="R3" s="28"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
@@ -1298,13 +1295,13 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="3">
         <v>39</v>
       </c>
@@ -1390,7 +1387,7 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="20">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1601,10 +1598,12 @@
       <c r="E10" s="19">
         <v>42</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="19">
+        <v>4</v>
+      </c>
       <c r="G10" s="20">
         <f>AVERAGE(G11:G13)</f>
-        <v>0.93333333333333324</v>
+        <v>1</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -1723,9 +1722,11 @@
       <c r="E13" s="19">
         <v>44</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="19">
+        <v>2</v>
+      </c>
       <c r="G13" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -1807,10 +1808,12 @@
       <c r="E15" s="19">
         <v>44</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="19">
+        <v>4</v>
+      </c>
       <c r="G15" s="20">
         <f>AVERAGE(G16:G18)</f>
-        <v>0.95000000000000007</v>
+        <v>1</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -1888,9 +1891,11 @@
       <c r="E17" s="19">
         <v>44</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="19">
+        <v>2</v>
+      </c>
       <c r="G17" s="20">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
@@ -2137,10 +2142,12 @@
       <c r="E23" s="19">
         <v>43</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="19">
+        <v>3</v>
+      </c>
       <c r="G23" s="20">
         <f>AVERAGE(G24:G26)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
@@ -2177,9 +2184,11 @@
       <c r="E24" s="19">
         <v>43</v>
       </c>
-      <c r="F24" s="19"/>
+      <c r="F24" s="19">
+        <v>2</v>
+      </c>
       <c r="G24" s="20">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2216,9 +2225,11 @@
       <c r="E25" s="19">
         <v>43</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
       <c r="G25" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
@@ -2255,9 +2266,11 @@
       <c r="E26" s="19">
         <v>43</v>
       </c>
-      <c r="F26" s="19"/>
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
       <c r="G26" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
@@ -2296,9 +2309,11 @@
       <c r="E27" s="19">
         <v>43</v>
       </c>
-      <c r="F27" s="19"/>
+      <c r="F27" s="19">
+        <v>2</v>
+      </c>
       <c r="G27" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
@@ -2339,7 +2354,7 @@
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="20">
-        <v>0.3</v>
+        <v>0.85</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>

</xml_diff>

<commit_message>
Added print in main to know that the file was saved. Changed how the timeout in GoToTarget works.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20C6A4E9-8285-429A-8BAC-37F8D2DA8CF0}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60E70FF7-0FE8-4D58-89FB-55449F9E4000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1169,7 +1171,7 @@
   <dimension ref="A1:AP32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1203,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="38" t="s">
@@ -1385,9 +1387,11 @@
       <c r="E5" s="19">
         <v>40</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="19">
+        <v>10</v>
+      </c>
       <c r="G5" s="20">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -2352,9 +2356,11 @@
       <c r="E28" s="19">
         <v>44</v>
       </c>
-      <c r="F28" s="19"/>
+      <c r="F28" s="19">
+        <v>5</v>
+      </c>
       <c r="G28" s="20">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>

</xml_diff>

<commit_message>
Added som external files. Cleaned up a bit of code in RRT. Nothing new.
</commit_message>
<xml_diff>
--- a/Documents/ProjectPlanner.xlsx
+++ b/Documents/ProjectPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_wal\OneDrive\Documents\Automatiseringsteknikk 3\Mekatronikk\Luretriks-Slange\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60E70FF7-0FE8-4D58-89FB-55449F9E4000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="114_{7FB3D701-8C10-416A-AE1D-684432DC9ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6E0012CC-6F75-4E39-954B-104CB8F1D24B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1170,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1391,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="20">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -2559,7 +2559,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="68" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>